<commit_message>
Last of known flat renames in this push.
</commit_message>
<xml_diff>
--- a/pk3/Textures/renamed/-=-Jul21Renamed.xlsx
+++ b/pk3/Textures/renamed/-=-Jul21Renamed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -322,6 +322,51 @@
   </si>
   <si>
     <t>_T100049</t>
+  </si>
+  <si>
+    <t>Z:\BLACK\lexicon\pk3\Textures\renamed\2\</t>
+  </si>
+  <si>
+    <t>CEIL1_2</t>
+  </si>
+  <si>
+    <t>_T100050</t>
+  </si>
+  <si>
+    <t>GATE1</t>
+  </si>
+  <si>
+    <t>_T100051</t>
+  </si>
+  <si>
+    <t>GATE2</t>
+  </si>
+  <si>
+    <t>_T100052</t>
+  </si>
+  <si>
+    <t>GATE3</t>
+  </si>
+  <si>
+    <t>_T100053</t>
+  </si>
+  <si>
+    <t>GATE4</t>
+  </si>
+  <si>
+    <t>_T100054</t>
+  </si>
+  <si>
+    <t>RROCK01</t>
+  </si>
+  <si>
+    <t>_T100055</t>
+  </si>
+  <si>
+    <t>RROCK02</t>
+  </si>
+  <si>
+    <t>_T100056</t>
   </si>
 </sst>
 </file>
@@ -728,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,6 +1197,78 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>